<commit_message>
Correcion de errores de la actualizacion de omar
</commit_message>
<xml_diff>
--- a/NominasMaecco/bin/Debug/Archivos/contador.xlsx
+++ b/NominasMaecco/bin/Debug/Archivos/contador.xlsx
@@ -916,7 +916,9 @@
     <tableColumn id="3" name="Column3" dataDxfId="10" totalsRowDxfId="3"/>
     <tableColumn id="4" name="Column4" dataDxfId="9" totalsRowDxfId="2"/>
     <tableColumn id="5" name="Column5" dataDxfId="8" totalsRowDxfId="1"/>
-    <tableColumn id="6" name="Column6" dataDxfId="7" totalsRowDxfId="0"/>
+    <tableColumn id="6" name="Column6" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="0">
+      <totalsRowFormula>V8-I32</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1213,10 +1215,10 @@
   <dimension ref="B2:V40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="G21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K33" sqref="K33"/>
+      <selection pane="bottomRight" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2087,7 +2089,10 @@
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
       <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
+      <c r="I33" s="29">
+        <f>V8-I32</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="23" t="s">

</xml_diff>

<commit_message>
Reporte del contador, variable comision, ajuste archivo reporte
</commit_message>
<xml_diff>
--- a/NominasMaecco/bin/Debug/Archivos/contador.xlsx
+++ b/NominasMaecco/bin/Debug/Archivos/contador.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
   <si>
     <t>SUELDO BASE</t>
   </si>
@@ -229,7 +229,19 @@
     <t>JUNIO</t>
   </si>
   <si>
-    <t>Comisión 2%</t>
+    <t>MAECCO</t>
+  </si>
+  <si>
+    <t>RETENCION 6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comisión </t>
+  </si>
+  <si>
+    <t>RET 6%</t>
+  </si>
+  <si>
+    <t>RETENCIONES</t>
   </si>
 </sst>
 </file>
@@ -240,7 +252,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +329,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -350,7 +369,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -430,6 +449,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -440,17 +470,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -489,6 +515,27 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="43" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -803,13 +850,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>10584</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>889000</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -907,8 +954,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table4345678" displayName="Table4345678" ref="C12:I33" totalsRowCount="1" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
-  <autoFilter ref="C12:I32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table4345678" displayName="Table4345678" ref="C12:I34" totalsRowCount="1" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
+  <autoFilter ref="C12:I33"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Column1" dataDxfId="13" totalsRowDxfId="6"/>
     <tableColumn id="7" name="Column12" dataDxfId="12" totalsRowDxfId="5"/>
@@ -917,7 +964,7 @@
     <tableColumn id="4" name="Column4" dataDxfId="9" totalsRowDxfId="2"/>
     <tableColumn id="5" name="Column5" dataDxfId="8" totalsRowDxfId="1"/>
     <tableColumn id="6" name="Column6" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="0">
-      <totalsRowFormula>V8-I32</totalsRowFormula>
+      <totalsRowFormula>Y8-I33</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1212,16 +1259,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="B2:V40"/>
+  <dimension ref="B2:Y41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="G21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I34" sqref="I34"/>
+      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" customWidth="1"/>
@@ -1232,912 +1279,1031 @@
     <col min="10" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" style="32" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" style="32" customWidth="1"/>
+    <col min="17" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="32" customWidth="1"/>
+    <col min="24" max="24" width="12" customWidth="1"/>
+    <col min="25" max="25" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="E2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="s">
+    <row r="2" spans="2:25" s="34" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="B2" s="33"/>
+      <c r="E2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="X2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="Y2" s="35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:22" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-    </row>
-    <row r="4" spans="2:22" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2">
+        <f>+L3+N3+O3+P3+Q3+R3+T3</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="2">
+        <f>+U3*0.16</f>
+        <v>0</v>
+      </c>
+      <c r="W3" s="29">
+        <f>+(N3+P3+Q3+T3)*6%</f>
+        <v>0</v>
+      </c>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2">
+        <f t="shared" ref="Y3:Y6" si="0">+U3+V3-W3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-    </row>
-    <row r="5" spans="2:22" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="29">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2">
+        <f t="shared" ref="U4:U6" si="1">+L4+N4+O4+P4+Q4+R4+T4</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="2">
+        <f t="shared" ref="V4:V6" si="2">+U4*0.16</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="29">
+        <f t="shared" ref="W4:W6" si="3">+(N4+P4+Q4+T4)*6%</f>
+        <v>0</v>
+      </c>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-    </row>
-    <row r="6" spans="2:22" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-    </row>
-    <row r="7" spans="2:22" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5">
+      <c r="D7" s="3"/>
+      <c r="E7" s="4">
         <f>SUM(E3:E6)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="5">
-        <f t="shared" ref="F7:U7" si="0">SUM(F3:F6)</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5">
+      <c r="F7" s="4">
+        <f t="shared" ref="F7:X7" si="4">SUM(F3:F6)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4">
         <f>SUM(M3:M6)</f>
         <v>0</v>
       </c>
-      <c r="N7" s="5">
-        <f>SUM(N3:N6)</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S7" s="5">
-        <f>SUM(S3:S6)</f>
-        <v>0</v>
-      </c>
-      <c r="T7" s="5">
-        <f>SUM(T3:T6)</f>
-        <v>0</v>
-      </c>
-      <c r="U7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V7" s="5">
+      <c r="N7" s="30">
+        <f t="shared" ref="N7" si="5">SUM(N3:N6)</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <f>SUM(O3:O6)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="30">
+        <f t="shared" ref="P7" si="6">SUM(P3:P6)</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U7" s="4">
+        <f>SUM(U3:U6)</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="4">
         <f>SUM(V3:V6)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
+      <c r="W7" s="30">
+        <f t="shared" ref="W7" si="7">SUM(W3:W6)</f>
+        <v>0</v>
+      </c>
+      <c r="X7" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="4">
+        <f>SUM(Y3:Y6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="18"/>
+      <c r="C8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7">
+      <c r="D8" s="24"/>
+      <c r="E8" s="37">
         <f>E7</f>
         <v>0</v>
       </c>
-      <c r="F8" s="7">
-        <f t="shared" ref="F8:U8" si="1">F7</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="7">
-        <f>N7</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V8" s="7">
-        <f>V7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="8" t="s">
+      <c r="F8" s="37">
+        <f t="shared" ref="F8:X8" si="8">F7</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="37">
+        <f>O7</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="38">
+        <f t="shared" ref="P8" si="9">P7</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="38">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X8" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="37">
+        <f>Y7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C12" s="3" t="s">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C14" s="10" t="s">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <f>E4</f>
         <v>0</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <f>E6</f>
         <v>0</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C15" s="10" t="s">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <f>F3</f>
         <v>0</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <f>F4</f>
         <v>0</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <f>F5</f>
         <v>0</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <f>F6</f>
         <v>0</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C16" s="10" t="s">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <f>G3</f>
         <v>0</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <f>G4</f>
         <v>0</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <f>G5</f>
         <v>0</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <f>G6</f>
         <v>0</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C17" s="10" t="s">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <f>H3</f>
         <v>0</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <f>H4</f>
         <v>0</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <f>H5</f>
         <v>0</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <f>H6</f>
         <v>0</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="2">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="10" t="s">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <f>J3</f>
         <v>0</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <f>J4</f>
         <v>0</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <f>J5</f>
         <v>0</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <f>J6</f>
         <v>0</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="10" t="s">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <f>I3</f>
         <v>0</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <f>I4</f>
         <v>0</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <f>I5</f>
         <v>0</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <f>I6</f>
         <v>0</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="10" t="s">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C20" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <f>K3</f>
         <v>0</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <f>K4</f>
         <v>0</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <f>K5</f>
         <v>0</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <f>K6</f>
         <v>0</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="12"/>
-      <c r="D21" s="12" t="s">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="3">
-        <f>U3</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <f>U4</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <f>U5</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
-        <f>U6</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="3">
+      <c r="E21" s="2">
+        <f>X3</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <f>X4</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <f>X5</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <f>X6</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="10" t="s">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C22" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="3">
-        <f>N3</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="3">
-        <f>N4</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="3">
-        <f>N5</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="3">
-        <f>N6</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="3">
+      <c r="E22" s="2">
+        <f>O3</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <f>O4</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <f>O5</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <f>O6</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="10">
         <f>L3</f>
         <v>0</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <f>L4</f>
         <v>0</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="10">
         <f>L5</f>
         <v>0</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="10">
         <f>L6</f>
         <v>0</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
-      <c r="J23" s="13"/>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="14" t="s">
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C24" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="16" t="s">
+      <c r="E24" s="24"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-    </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="17" t="s">
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="29"/>
+    </row>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="16"/>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="14" t="s">
+      <c r="E25" s="24"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C26" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="26"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="16"/>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C27" s="17" t="s">
+      <c r="E26" s="24"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C27" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="26"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="16"/>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C28" s="10" t="s">
+      <c r="E27" s="24"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C28" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="12">
-        <f>Q3</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="3">
-        <f>Q4</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="3">
-        <f>Q5</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="12">
-        <f>Q6</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="3">
+      <c r="E28" s="10">
+        <f>S3</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <f>S4</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <f>S5</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="10">
+        <f>S6</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
-      <c r="J28" s="16"/>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C29" s="10" t="s">
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C29" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="19">
-        <f>O3+P3</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="19">
-        <f>O4+P4</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="19">
-        <f>O5+P5</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="19">
-        <f>O6+P6</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="19">
+      <c r="D29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="17">
+        <f>Q3+R3</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="17">
+        <f>Q4+R4</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="17">
+        <f>Q5+R5</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="17">
+        <f>Q6+R6</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="17">
         <f>SUM(Table4345678[[#This Row],[Column2]:[Column5]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C30" s="3"/>
-      <c r="D30" s="3" t="s">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <f>SUBTOTAL(109,E13:E29)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <f>SUBTOTAL(109,F13:F29)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="2">
         <f>SUBTOTAL(109,G13:G29)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="2">
         <f>SUBTOTAL(109,H13:H29)</f>
         <v>0</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="2">
         <f>SUBTOTAL(109,I13:I29)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3" t="s">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <f>+E30*0.16</f>
         <v>0</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <f>+F30*0.16</f>
         <v>0</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="2">
         <f>+G30*0.16</f>
         <v>0</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="2">
         <f>+H30*0.16</f>
         <v>0</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="2">
         <f>+I30*0.16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="20"/>
-      <c r="D32" s="20" t="s">
+    <row r="32" spans="3:16" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="29"/>
+      <c r="D32" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29">
+        <f>+X4</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29">
+        <f>+Table4345678[[#This Row],[Column3]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="18"/>
+      <c r="D33" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E33" s="19">
         <f>+E30+E31</f>
         <v>0</v>
       </c>
-      <c r="F32" s="21">
-        <f>+F30+F31</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="21">
+      <c r="F33" s="19">
+        <f>+F30+F31-F32</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="19">
         <f>+G30+G31</f>
         <v>0</v>
       </c>
-      <c r="H32" s="21">
+      <c r="H33" s="19">
         <f>+H30+H31</f>
         <v>0</v>
       </c>
-      <c r="I32" s="21">
-        <f>+I30+I31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29">
-        <f>V8-I32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="23" t="s">
+      <c r="I33" s="19">
+        <f>+I30+I31-I32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27">
+        <f>Y8-I33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C35" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="24"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C36" s="25" t="s">
+      <c r="D35" s="20"/>
+      <c r="E35" s="22"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C37" s="23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C37" s="14" t="s">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C38" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D38" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="17" t="s">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D39" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="14" t="s">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C40" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D40" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="17" t="s">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D41" s="16" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>